<commit_message>
Small modifications in the template excel file.
</commit_message>
<xml_diff>
--- a/examples/template_input.xlsx
+++ b/examples/template_input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\OneDrive\Work\TaborLab\Code\fc\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\castillohair\Documents\Rice\Lab\Programs\fc\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="beads" sheetId="2" r:id="rId1"/>
@@ -58,30 +58,9 @@
     <t>To use this sheet, fill out columns as specified, then delete the instructions (rows 2,3)</t>
   </si>
   <si>
-    <t>The path to the bead FCS file associated with this data relative to the location of this document. Example: "FCFiles/beads_001.fcs". Only required if using Mef Transform on this data</t>
-  </si>
-  <si>
     <t>FL2 Peaks</t>
   </si>
   <si>
-    <t>The fraction of events to include in the density gate of the FSC-SSC plot. Accepts values 0-1. Suggested fraction of "0.3".</t>
-  </si>
-  <si>
-    <t>The clustering method to use it identify bead peaks. Suggested input of "gmm".</t>
-  </si>
-  <si>
-    <t>The channels to utilize when clustering the beads in comma seperated value format. It is suggested that you include all channels which do not clip off bead peaks entirely. Example input: "FL1, FL2, FL3"</t>
-  </si>
-  <si>
-    <t>The manufacturer supplied peaks of the beads in comma sperated value format. The first peak should be None if the beads contain autofluoresence. The most recent (8/19/2015) beads received by the Tabor Lab had the following peaks: "None, 792, 2079, 6588, 16471, 47497, 137049, 271647"</t>
-  </si>
-  <si>
-    <t>The manufacturer supplied peaks of the beads in comma sperated value format. The first peak should be None if the beads contain autofluoresence.</t>
-  </si>
-  <si>
-    <t>The manufacturer supplied peaks of the beads in comma sperated value format. The first peak should be None if the beads contain autofluoresence. The most recent (8/19/2015) beads received by the Tabor Lab had the following peaks: "None, 1614, 4035, 12025, 31896, 95682, 353225, 1077421"</t>
-  </si>
-  <si>
     <t>The path to the FCS file representing beads relative to the location of this document. Example: "FCFiles/beads_001.fcs"</t>
   </si>
   <si>
@@ -89,6 +68,27 @@
   </si>
   <si>
     <t>Fraction of events in the density gate applied to the FSS SSC channels which are kept. Accepts values 0-1. Suggested values of "0.1" to "0.3".</t>
+  </si>
+  <si>
+    <t>The manufacturer supplied values of the beads' fluroescence for the channel FL2 in comma sperated value format, from lowest to highest. Normally, a group of beads with no fluorophore is included, in which case its fluorescence value should be specified as zero. If a particular cluster of beads should be excluded from the analysis, the string "None" can be provided instead of the numerical value.</t>
+  </si>
+  <si>
+    <t>The manufacturer supplied values of the beads' fluroescence for the channel FL3 in comma sperated value format, from lowest to highest. Normally, a group of beads with no fluorophore is included, in which case its fluorescence value should be specified as zero. If a particular cluster of beads should be excluded from the analysis, the string "None" can be provided instead of the numerical value.</t>
+  </si>
+  <si>
+    <t>The manufacturer supplied values of the beads' fluroescence for the channel FL1 in comma sperated value format, from lowest to highest. Normally, a group of beads with no fluorophore is included, in which case its fluorescence value should be specified as zero. If a particular cluster of beads should be excluded from the analysis, the string "None" can be provided instead of the numerical value. Example: "0, 792, 2079, 6588, 16471, 47497, 137049, 271647"</t>
+  </si>
+  <si>
+    <t>The channels to utilize when clustering beads peaks, in comma seperated value format. It is suggested that you include three fluorescence channels that do not clip off bead peaks entirely. Example input: "FL1, FL2, FL3"</t>
+  </si>
+  <si>
+    <t>The fraction of events to include when performing density gating on the FSC-SSC plot. Accepts values 0-1. Suggested fraction of "0.3".</t>
+  </si>
+  <si>
+    <t>The clustering method to use to identify bead peaks. Suggested input of "gmm".</t>
+  </si>
+  <si>
+    <t>The path to the bead FCS file associated with this data relative to the location of this document. Example: "FCFiles/beads_001.fcs". Only required if transforming fluorescence values to MEF units.</t>
   </si>
 </sst>
 </file>
@@ -463,21 +463,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -485,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -500,30 +500,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -548,19 +548,19 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -580,27 +580,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="208" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="207.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>

</xml_diff>